<commit_message>
Added Status column to API so to see what's ready.
</commit_message>
<xml_diff>
--- a/middlelayer/API.xlsx
+++ b/middlelayer/API.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>ACCESSION_SEARCH</t>
   </si>
@@ -172,13 +172,19 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +203,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -222,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -233,6 +247,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,7 +523,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -513,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +544,7 @@
     <col min="5" max="5" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -542,8 +560,11 @@
       <c r="E1" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -559,8 +580,11 @@
       <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -577,7 +601,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -594,7 +618,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -611,7 +635,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -628,7 +652,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -645,7 +669,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -660,7 +684,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -675,7 +699,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -689,8 +713,11 @@
         <v>12</v>
       </c>
       <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F10" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -704,8 +731,11 @@
         <v>14</v>
       </c>
       <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -714,7 +744,7 @@
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -725,7 +755,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>46</v>
       </c>
@@ -736,7 +766,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Updated status; changes to intron/exon
</commit_message>
<xml_diff>
--- a/middlelayer/API.xlsx
+++ b/middlelayer/API.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>ACCESSION_SEARCH</t>
   </si>
@@ -93,9 +93,6 @@
     <t>1 array of concatenated product names, id and location</t>
   </si>
   <si>
-    <t>DNA sequence</t>
-  </si>
-  <si>
     <t>Coding sequence and amino acids sequence</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>1 string and 1 hash</t>
   </si>
   <si>
-    <t>2 arrays : 1 of start positions, 1 of end positions of restrictions sites. (It could be an hash).</t>
-  </si>
-  <si>
     <t>1 array of accessions</t>
   </si>
   <si>
@@ -168,25 +162,25 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Does not need a function</t>
-  </si>
-  <si>
-    <t>Does not need a function.</t>
-  </si>
-  <si>
     <t>The coding sequence; concatenated exons (1 string).</t>
   </si>
   <si>
-    <t>The front end can do this task with 2 lines of code by only having the full DNA sequence and an hash of exons position. We aleady have SQL fnctions retrieving those for the front end to use.  The front end just need to place tags around each exon subtring.</t>
-  </si>
-  <si>
     <t>DOne</t>
   </si>
   <si>
-    <t>This task can be completed by only giving the front end the full DNA sequence and an hash of exons positions/length; both retrievable with queries; all the front end needs is to know which sbstring within the main string to highligh; same we decided to do for the restriction sites task. Code for the front layer:                                                                 foreach my $key (keys %exons)   {
-   substr($sequence, $key, $exons{$key}) = "&lt;div&gt;" . substr($sequence,    $key, $exons{$key} ) . "&lt;/div&gt;";
-}
-print "&lt;p&gt; $sequence &lt;/p&gt;";</t>
+    <t>Work in progress</t>
+  </si>
+  <si>
+    <t>Does probably not need a function.</t>
+  </si>
+  <si>
+    <t>Does probably not need a function</t>
+  </si>
+  <si>
+    <t>DNA sequence and exons positions</t>
+  </si>
+  <si>
+    <t>Task different from what we thought. Done. Please se module ezymes.pm</t>
   </si>
 </sst>
 </file>
@@ -532,7 +526,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -542,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,19 +552,19 @@
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -587,30 +581,30 @@
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -618,19 +612,19 @@
         <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -638,19 +632,19 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -658,19 +652,19 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -678,39 +672,39 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="F7" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="B8" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -718,17 +712,17 @@
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -736,7 +730,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
@@ -746,7 +740,7 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -754,7 +748,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>4</v>
@@ -764,7 +758,7 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -789,7 +783,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -798,21 +792,21 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>